<commit_message>
fixed test file 7
</commit_message>
<xml_diff>
--- a/test_initial_states/initial_state_7.xlsx
+++ b/test_initial_states/initial_state_7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/aaron_t_wong_vanderbilt_edu/Documents/Desktop/initial_states/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\aaronwong\code\ai_project\test_initial_states\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{1F6677A5-8E55-470C-908F-28301DFD6290}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D8523B0D-649A-4D10-A09C-EAE05371EEB6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E999AB-C9B4-4925-82C7-F63E099BA8F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13065" yWindow="750" windowWidth="23025" windowHeight="15555" xr2:uid="{65B8699D-C102-4177-9EDB-4160093663D6}"/>
+    <workbookView xWindow="14415" yWindow="1320" windowWidth="23025" windowHeight="15555" xr2:uid="{65B8699D-C102-4177-9EDB-4160093663D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C2" sqref="C2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,43 +567,56 @@
         <v>100</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <f t="shared" ref="C2" si="0">1.5*B2</f>
+        <v>150</v>
       </c>
       <c r="D2" s="1">
-        <v>15</v>
+        <f t="shared" ref="D2" si="1">1*B2</f>
+        <v>100</v>
       </c>
       <c r="E2" s="2">
-        <v>100</v>
+        <f t="shared" ref="E2" si="2">B2*6</f>
+        <v>600</v>
       </c>
       <c r="F2" s="2">
-        <v>300</v>
+        <f t="shared" ref="F2" si="3">B2*50</f>
+        <v>5000</v>
       </c>
       <c r="G2" s="2">
-        <v>400</v>
+        <f t="shared" ref="G2" si="4">B2*50</f>
+        <v>5000</v>
       </c>
       <c r="H2" s="2">
-        <v>30</v>
+        <f t="shared" ref="H2" si="5">B2*300</f>
+        <v>30000</v>
       </c>
       <c r="I2" s="1">
-        <v>300</v>
+        <f t="shared" ref="I2" si="6">B2*33</f>
+        <v>3300</v>
       </c>
       <c r="J2" s="1">
+        <f t="shared" ref="J2" si="7">B2*2.5</f>
+        <v>250</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" ref="K2" si="8">B2*1.5</f>
+        <v>150</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" ref="L2" si="9">B2*0.4</f>
         <v>40</v>
       </c>
-      <c r="K2" s="1">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1">
-        <v>4</v>
-      </c>
       <c r="M2" s="1">
-        <v>111</v>
+        <f t="shared" ref="M2" si="10">B2*10</f>
+        <v>1000</v>
       </c>
       <c r="N2" s="1">
-        <v>50</v>
+        <f t="shared" ref="N2" si="11">B2*10</f>
+        <v>1000</v>
       </c>
       <c r="O2" s="1">
-        <v>5</v>
+        <f t="shared" ref="O2" si="12">B2*1</f>
+        <v>100</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -638,55 +651,55 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C6" si="0">1.5*B3</f>
+        <f t="shared" ref="C3:C6" si="13">1.5*B3</f>
         <v>150</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D6" si="1">1*B3</f>
+        <f t="shared" ref="D3:D6" si="14">1*B3</f>
         <v>100</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E6" si="2">B3*6</f>
+        <f t="shared" ref="E3:E6" si="15">B3*6</f>
         <v>600</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F6" si="3">B3*50</f>
+        <f t="shared" ref="F3:F6" si="16">B3*50</f>
         <v>5000</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G6" si="4">B3*50</f>
+        <f t="shared" ref="G3:G6" si="17">B3*50</f>
         <v>5000</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H6" si="5">B3*300</f>
+        <f t="shared" ref="H3:H6" si="18">B3*300</f>
         <v>30000</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I6" si="6">B3*33</f>
+        <f t="shared" ref="I3:I6" si="19">B3*33</f>
         <v>3300</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J6" si="7">B3*2.5</f>
+        <f t="shared" ref="J3:J6" si="20">B3*2.5</f>
         <v>250</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K6" si="8">B3*1.5</f>
+        <f t="shared" ref="K3:K6" si="21">B3*1.5</f>
         <v>150</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="9">B3*0.4</f>
+        <f t="shared" ref="L3:L6" si="22">B3*0.4</f>
         <v>40</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M6" si="10">B3*10</f>
+        <f t="shared" ref="M3:M6" si="23">B3*10</f>
         <v>1000</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N6" si="11">B3*10</f>
+        <f t="shared" ref="N3:N6" si="24">B3*10</f>
         <v>1000</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" ref="O3:O6" si="12">B3*1</f>
+        <f t="shared" ref="O3:O6" si="25">B3*1</f>
         <v>100</v>
       </c>
       <c r="P3" s="1">
@@ -722,55 +735,55 @@
         <v>100</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>150</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>600</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>5000</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>5000</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>30000</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>3300</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>250</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>150</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>40</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>1000</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1000</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>100</v>
       </c>
       <c r="P4" s="1">
@@ -806,55 +819,55 @@
         <v>100</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>150</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>600</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>5000</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>5000</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>30000</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>3300</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>250</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>150</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>40</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>1000</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1000</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>100</v>
       </c>
       <c r="P5" s="1">
@@ -890,55 +903,55 @@
         <v>100</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="13"/>
         <v>150</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>600</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>5000</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>5000</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>30000</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>3300</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>250</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>150</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>40</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>1000</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1000</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>100</v>
       </c>
       <c r="P6" s="1">

</xml_diff>

<commit_message>
Revert "fixed test file 7"
This reverts commit 59ce1666d3f3cf0a1833128fd7195f8c87c39605.
</commit_message>
<xml_diff>
--- a/test_initial_states/initial_state_7.xlsx
+++ b/test_initial_states/initial_state_7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\aaronwong\code\ai_project\test_initial_states\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/aaron_t_wong_vanderbilt_edu/Documents/Desktop/initial_states/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E999AB-C9B4-4925-82C7-F63E099BA8F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{1F6677A5-8E55-470C-908F-28301DFD6290}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D8523B0D-649A-4D10-A09C-EAE05371EEB6}"/>
   <bookViews>
-    <workbookView xWindow="14415" yWindow="1320" windowWidth="23025" windowHeight="15555" xr2:uid="{65B8699D-C102-4177-9EDB-4160093663D6}"/>
+    <workbookView xWindow="13065" yWindow="750" windowWidth="23025" windowHeight="15555" xr2:uid="{65B8699D-C102-4177-9EDB-4160093663D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:O2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,56 +567,43 @@
         <v>100</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2" si="0">1.5*B2</f>
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2" si="1">1*B2</f>
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2" si="2">B2*6</f>
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" ref="F2" si="3">B2*50</f>
-        <v>5000</v>
+        <v>300</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" ref="G2" si="4">B2*50</f>
-        <v>5000</v>
+        <v>400</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ref="H2" si="5">B2*300</f>
-        <v>30000</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2" si="6">B2*33</f>
-        <v>3300</v>
+        <v>300</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" ref="J2" si="7">B2*2.5</f>
-        <v>250</v>
+        <v>40</v>
       </c>
       <c r="K2" s="1">
-        <f t="shared" ref="K2" si="8">B2*1.5</f>
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="L2" s="1">
-        <f t="shared" ref="L2" si="9">B2*0.4</f>
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1">
-        <f t="shared" ref="M2" si="10">B2*10</f>
-        <v>1000</v>
+        <v>111</v>
       </c>
       <c r="N2" s="1">
-        <f t="shared" ref="N2" si="11">B2*10</f>
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="O2" s="1">
-        <f t="shared" ref="O2" si="12">B2*1</f>
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -651,55 +638,55 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C6" si="13">1.5*B3</f>
+        <f t="shared" ref="C3:C6" si="0">1.5*B3</f>
         <v>150</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D6" si="14">1*B3</f>
+        <f t="shared" ref="D3:D6" si="1">1*B3</f>
         <v>100</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E6" si="15">B3*6</f>
+        <f t="shared" ref="E3:E6" si="2">B3*6</f>
         <v>600</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F6" si="16">B3*50</f>
+        <f t="shared" ref="F3:F6" si="3">B3*50</f>
         <v>5000</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G6" si="17">B3*50</f>
+        <f t="shared" ref="G3:G6" si="4">B3*50</f>
         <v>5000</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H6" si="18">B3*300</f>
+        <f t="shared" ref="H3:H6" si="5">B3*300</f>
         <v>30000</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I6" si="19">B3*33</f>
+        <f t="shared" ref="I3:I6" si="6">B3*33</f>
         <v>3300</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J6" si="20">B3*2.5</f>
+        <f t="shared" ref="J3:J6" si="7">B3*2.5</f>
         <v>250</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K6" si="21">B3*1.5</f>
+        <f t="shared" ref="K3:K6" si="8">B3*1.5</f>
         <v>150</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L6" si="22">B3*0.4</f>
+        <f t="shared" ref="L3:L6" si="9">B3*0.4</f>
         <v>40</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M6" si="23">B3*10</f>
+        <f t="shared" ref="M3:M6" si="10">B3*10</f>
         <v>1000</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N6" si="24">B3*10</f>
+        <f t="shared" ref="N3:N6" si="11">B3*10</f>
         <v>1000</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" ref="O3:O6" si="25">B3*1</f>
+        <f t="shared" ref="O3:O6" si="12">B3*1</f>
         <v>100</v>
       </c>
       <c r="P3" s="1">
@@ -735,55 +722,55 @@
         <v>100</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="5"/>
         <v>30000</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="6"/>
         <v>3300</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="8"/>
         <v>150</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>1000</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>1000</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="P4" s="1">
@@ -819,55 +806,55 @@
         <v>100</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="5"/>
         <v>30000</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="6"/>
         <v>3300</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="8"/>
         <v>150</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>1000</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>1000</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="P5" s="1">
@@ -903,55 +890,55 @@
         <v>100</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="5"/>
         <v>30000</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="6"/>
         <v>3300</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="7"/>
         <v>250</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="8"/>
         <v>150</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="10"/>
         <v>1000</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="11"/>
         <v>1000</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="P6" s="1">

</xml_diff>